<commit_message>
update omnetpp.ini, analysis and notes
-added factors calibration configuration, analysis charts and notes
</commit_message>
<xml_diff>
--- a/Analysis/verification/monotonicity_test/minions/mean_response_time/test_100_repetitions.xlsx
+++ b/Analysis/verification/monotonicity_test/minions/mean_response_time/test_100_repetitions.xlsx
@@ -11,8 +11,8 @@
     <sheet name="Sheet1" sheetId="1" state="visible" r:id="rId2"/>
   </sheets>
   <definedNames>
-    <definedName function="false" hidden="true" localSheetId="0" name="_xlnm._FilterDatabase" vbProcedure="false">Sheet1!$B$426:$I$526</definedName>
-    <definedName function="false" hidden="false" localSheetId="0" name="_xlnm._FilterDatabase" vbProcedure="false">Sheet1!$B$62:$I$72</definedName>
+    <definedName function="false" hidden="true" localSheetId="0" name="_xlnm._FilterDatabase" vbProcedure="false">Sheet1!$B$62:$I$72</definedName>
+    <definedName function="false" hidden="false" localSheetId="0" name="_xlnm._FilterDatabase" vbProcedure="false">Sheet1!$B$426:$I$526</definedName>
   </definedNames>
   <calcPr iterateCount="100" refMode="A1" iterate="false" iterateDelta="0.001"/>
   <extLst>
@@ -269,7 +269,7 @@
 </styleSheet>
 </file>
 
-<file path=xl/charts/chart7.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/charts/chart4.xml><?xml version="1.0" encoding="utf-8"?>
 <c:chartSpace xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
   <c:lang val="en-US"/>
   <c:roundedCorners val="0"/>
@@ -357,6 +357,7 @@
                   </a:pPr>
                 </a:p>
               </c:txPr>
+              <c:dLblPos val="outEnd"/>
               <c:showLegendKey val="0"/>
               <c:showVal val="0"/>
               <c:showCatName val="0"/>
@@ -375,6 +376,7 @@
                 </a:pPr>
               </a:p>
             </c:txPr>
+            <c:dLblPos val="outEnd"/>
             <c:showLegendKey val="0"/>
             <c:showVal val="0"/>
             <c:showCatName val="0"/>
@@ -468,6 +470,7 @@
                 </a:pPr>
               </a:p>
             </c:txPr>
+            <c:dLblPos val="outEnd"/>
             <c:showLegendKey val="0"/>
             <c:showVal val="0"/>
             <c:showCatName val="0"/>
@@ -561,6 +564,7 @@
                 </a:pPr>
               </a:p>
             </c:txPr>
+            <c:dLblPos val="outEnd"/>
             <c:showLegendKey val="0"/>
             <c:showVal val="0"/>
             <c:showCatName val="0"/>
@@ -654,6 +658,7 @@
                 </a:pPr>
               </a:p>
             </c:txPr>
+            <c:dLblPos val="outEnd"/>
             <c:showLegendKey val="0"/>
             <c:showVal val="0"/>
             <c:showCatName val="0"/>
@@ -747,6 +752,7 @@
                 </a:pPr>
               </a:p>
             </c:txPr>
+            <c:dLblPos val="outEnd"/>
             <c:showLegendKey val="0"/>
             <c:showVal val="0"/>
             <c:showCatName val="0"/>
@@ -807,11 +813,11 @@
         </c:ser>
         <c:gapWidth val="500"/>
         <c:overlap val="-100"/>
-        <c:axId val="41978460"/>
-        <c:axId val="1368414"/>
+        <c:axId val="91907862"/>
+        <c:axId val="43179705"/>
       </c:barChart>
       <c:catAx>
-        <c:axId val="41978460"/>
+        <c:axId val="91907862"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -867,7 +873,7 @@
             </a:pPr>
           </a:p>
         </c:txPr>
-        <c:crossAx val="1368414"/>
+        <c:crossAx val="43179705"/>
         <c:crosses val="autoZero"/>
         <c:auto val="1"/>
         <c:lblAlgn val="ctr"/>
@@ -875,7 +881,7 @@
         <c:noMultiLvlLbl val="0"/>
       </c:catAx>
       <c:valAx>
-        <c:axId val="1368414"/>
+        <c:axId val="43179705"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -918,7 +924,7 @@
             </a:ln>
           </c:spPr>
         </c:title>
-        <c:numFmt formatCode="General" sourceLinked="1"/>
+        <c:numFmt formatCode="General" sourceLinked="0"/>
         <c:majorTickMark val="out"/>
         <c:minorTickMark val="none"/>
         <c:tickLblPos val="nextTo"/>
@@ -940,7 +946,7 @@
             </a:pPr>
           </a:p>
         </c:txPr>
-        <c:crossAx val="41978460"/>
+        <c:crossAx val="91907862"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="between"/>
       </c:valAx>
@@ -991,7 +997,7 @@
     <a:solidFill>
       <a:srgbClr val="ffffff"/>
     </a:solidFill>
-    <a:ln>
+    <a:ln w="9360">
       <a:noFill/>
     </a:ln>
   </c:spPr>
@@ -1009,9 +1015,9 @@
     </xdr:from>
     <xdr:to>
       <xdr:col>21</xdr:col>
-      <xdr:colOff>416520</xdr:colOff>
+      <xdr:colOff>408960</xdr:colOff>
       <xdr:row>21</xdr:row>
-      <xdr:rowOff>70200</xdr:rowOff>
+      <xdr:rowOff>76680</xdr:rowOff>
     </xdr:to>
     <xdr:graphicFrame>
       <xdr:nvGraphicFramePr>
@@ -1019,8 +1025,8 @@
         <xdr:cNvGraphicFramePr/>
       </xdr:nvGraphicFramePr>
       <xdr:xfrm>
-        <a:off x="16053120" y="963000"/>
-        <a:ext cx="5759640" cy="3239640"/>
+        <a:off x="16066440" y="963000"/>
+        <a:ext cx="5760720" cy="3246120"/>
       </xdr:xfrm>
       <a:graphic>
         <a:graphicData uri="http://schemas.openxmlformats.org/drawingml/2006/chart">
@@ -1041,15 +1047,15 @@
   <dimension ref="A1:L526"/>
   <sheetViews>
     <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="J1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="A2" activeCellId="0" sqref="A2"/>
+      <selection pane="topLeft" activeCell="M8" activeCellId="0" sqref="M8"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="11.55078125" defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
+  <sheetFormatPr defaultColWidth="11.5703125" defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
   <cols>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1" min="1" style="0" width="36.26"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="2" min="2" style="0" width="27.09"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="5" min="5" style="0" width="13.75"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="6" min="6" style="0" width="30.01"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="6" min="6" style="0" width="30.02"/>
   </cols>
   <sheetData>
     <row r="1" customFormat="false" ht="69.4" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
@@ -2460,25 +2466,25 @@
       </c>
     </row>
     <row r="62" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="B62" s="0" t="s">
-        <v>11</v>
-      </c>
-      <c r="C62" s="0" t="s">
+      <c r="B62" s="2" t="s">
+        <v>11</v>
+      </c>
+      <c r="C62" s="2" t="s">
         <v>12</v>
       </c>
-      <c r="D62" s="0" t="n">
+      <c r="D62" s="2" t="n">
         <v>59</v>
       </c>
-      <c r="E62" s="0" t="s">
-        <v>13</v>
-      </c>
-      <c r="F62" s="0" t="s">
-        <v>14</v>
-      </c>
-      <c r="G62" s="0" t="n">
+      <c r="E62" s="2" t="s">
+        <v>13</v>
+      </c>
+      <c r="F62" s="2" t="s">
+        <v>14</v>
+      </c>
+      <c r="G62" s="2" t="n">
         <v>990</v>
       </c>
-      <c r="H62" s="0" t="n">
+      <c r="H62" s="2" t="n">
         <v>15.4489878918162</v>
       </c>
     </row>
@@ -12780,7 +12786,7 @@
       </c>
     </row>
   </sheetData>
-  <autoFilter ref="B426:I526"/>
+  <autoFilter ref="B62:I72"/>
   <printOptions headings="false" gridLines="false" gridLinesSet="true" horizontalCentered="false" verticalCentered="false"/>
   <pageMargins left="0.7875" right="0.7875" top="1.05277777777778" bottom="1.05277777777778" header="0.7875" footer="0.7875"/>
   <pageSetup paperSize="9" scale="100" firstPageNumber="1" fitToWidth="1" fitToHeight="1" pageOrder="downThenOver" orientation="portrait" blackAndWhite="false" draft="false" cellComments="none" useFirstPageNumber="true" horizontalDpi="300" verticalDpi="300" copies="1"/>

</xml_diff>

<commit_message>
factor calibration with repetitions
made factors calibration for minion and bosses with 30 repetitions (only missing the factors calibration for recover rate)
</commit_message>
<xml_diff>
--- a/Analysis/verification/monotonicity_test/minions/mean_response_time/test_100_repetitions.xlsx
+++ b/Analysis/verification/monotonicity_test/minions/mean_response_time/test_100_repetitions.xlsx
@@ -11,8 +11,8 @@
     <sheet name="Sheet1" sheetId="1" state="visible" r:id="rId2"/>
   </sheets>
   <definedNames>
-    <definedName function="false" hidden="true" localSheetId="0" name="_xlnm._FilterDatabase" vbProcedure="false">Sheet1!$B$62:$I$72</definedName>
-    <definedName function="false" hidden="false" localSheetId="0" name="_xlnm._FilterDatabase" vbProcedure="false">Sheet1!$B$426:$I$526</definedName>
+    <definedName function="false" hidden="true" localSheetId="0" name="_xlnm._FilterDatabase" vbProcedure="false">Sheet1!$B$426:$I$526</definedName>
+    <definedName function="false" hidden="false" localSheetId="0" name="_xlnm._FilterDatabase" vbProcedure="false">Sheet1!$B$62:$I$72</definedName>
   </definedNames>
   <calcPr iterateCount="100" refMode="A1" iterate="false" iterateDelta="0.001"/>
   <extLst>
@@ -269,7 +269,7 @@
 </styleSheet>
 </file>
 
-<file path=xl/charts/chart4.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/charts/chart1.xml><?xml version="1.0" encoding="utf-8"?>
 <c:chartSpace xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
   <c:lang val="en-US"/>
   <c:roundedCorners val="0"/>
@@ -813,11 +813,11 @@
         </c:ser>
         <c:gapWidth val="500"/>
         <c:overlap val="-100"/>
-        <c:axId val="91907862"/>
-        <c:axId val="43179705"/>
+        <c:axId val="3356088"/>
+        <c:axId val="26798820"/>
       </c:barChart>
       <c:catAx>
-        <c:axId val="91907862"/>
+        <c:axId val="3356088"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -873,7 +873,7 @@
             </a:pPr>
           </a:p>
         </c:txPr>
-        <c:crossAx val="43179705"/>
+        <c:crossAx val="26798820"/>
         <c:crosses val="autoZero"/>
         <c:auto val="1"/>
         <c:lblAlgn val="ctr"/>
@@ -881,7 +881,7 @@
         <c:noMultiLvlLbl val="0"/>
       </c:catAx>
       <c:valAx>
-        <c:axId val="43179705"/>
+        <c:axId val="26798820"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -946,7 +946,7 @@
             </a:pPr>
           </a:p>
         </c:txPr>
-        <c:crossAx val="91907862"/>
+        <c:crossAx val="3356088"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="between"/>
       </c:valAx>
@@ -1015,9 +1015,9 @@
     </xdr:from>
     <xdr:to>
       <xdr:col>21</xdr:col>
-      <xdr:colOff>408960</xdr:colOff>
+      <xdr:colOff>408600</xdr:colOff>
       <xdr:row>21</xdr:row>
-      <xdr:rowOff>76680</xdr:rowOff>
+      <xdr:rowOff>76320</xdr:rowOff>
     </xdr:to>
     <xdr:graphicFrame>
       <xdr:nvGraphicFramePr>
@@ -1025,8 +1025,8 @@
         <xdr:cNvGraphicFramePr/>
       </xdr:nvGraphicFramePr>
       <xdr:xfrm>
-        <a:off x="16066440" y="963000"/>
-        <a:ext cx="5760720" cy="3246120"/>
+        <a:off x="16079760" y="963000"/>
+        <a:ext cx="5769360" cy="3245760"/>
       </xdr:xfrm>
       <a:graphic>
         <a:graphicData uri="http://schemas.openxmlformats.org/drawingml/2006/chart">
@@ -1046,11 +1046,11 @@
   </sheetPr>
   <dimension ref="A1:L526"/>
   <sheetViews>
-    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="J1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="M8" activeCellId="0" sqref="M8"/>
+    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
+      <selection pane="topLeft" activeCell="L4" activeCellId="0" sqref="L4"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="11.5703125" defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
+  <sheetFormatPr defaultColWidth="11.58984375" defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
   <cols>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1" min="1" style="0" width="36.26"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="2" min="2" style="0" width="27.09"/>
@@ -1122,7 +1122,7 @@
         <v>15.6390253525561</v>
       </c>
       <c r="K3" s="0" t="n">
-        <f aca="false">STDEV(H3:H102)</f>
+        <f aca="false">SQRT(_xlfn.VAR.S(H3:H102))</f>
         <v>8.66333796041896</v>
       </c>
       <c r="L3" s="0" t="n">
@@ -12786,7 +12786,7 @@
       </c>
     </row>
   </sheetData>
-  <autoFilter ref="B62:I72"/>
+  <autoFilter ref="B426:I526"/>
   <printOptions headings="false" gridLines="false" gridLinesSet="true" horizontalCentered="false" verticalCentered="false"/>
   <pageMargins left="0.7875" right="0.7875" top="1.05277777777778" bottom="1.05277777777778" header="0.7875" footer="0.7875"/>
   <pageSetup paperSize="9" scale="100" firstPageNumber="1" fitToWidth="1" fitToHeight="1" pageOrder="downThenOver" orientation="portrait" blackAndWhite="false" draft="false" cellComments="none" useFirstPageNumber="true" horizontalDpi="300" verticalDpi="300" copies="1"/>

</xml_diff>